<commit_message>
Published state of ETDataset for deploy February 2025
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_hydrogen_solar_pv_solar_radiation.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_hydrogen_solar_pv_solar_radiation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10119"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roosdekok/code/etdataset/nodes_source_analyses/energy/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyradehaan/github/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE5B49A-037F-B94B-8D53-3687AD5C62BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDFF268-A29A-7143-A28D-3715A55BA93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4800" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="186">
   <si>
     <t>Source</t>
   </si>
@@ -349,9 +349,6 @@
     <t>Author</t>
   </si>
   <si>
-    <t>Maria Tsagkaraki</t>
-  </si>
-  <si>
     <t>Legend</t>
   </si>
   <si>
@@ -787,6 +784,12 @@
   </si>
   <si>
     <t>energy_power_solar_pv_solar_radiation.ad</t>
+  </si>
+  <si>
+    <t>Kyra de Haan</t>
+  </si>
+  <si>
+    <t>Quintel assumption: this attribute has no working purpose for modelling of this technology and is therefore set to 1.0</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1739,7 @@
     <xf numFmtId="164" fontId="41" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="41" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2104,6 +2107,7 @@
     <xf numFmtId="0" fontId="39" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="310">
     <cellStyle name="Comma" xfId="308" builtinId="3"/>
@@ -3365,16 +3369,16 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="62" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="62" customWidth="1"/>
     <col min="2" max="2" width="12" style="28" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="28" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="28"/>
+    <col min="3" max="3" width="38.5" style="28" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="60" customFormat="1">
@@ -3400,7 +3404,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3409,7 +3413,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3434,7 +3438,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="4"/>
       <c r="B9" s="93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="94"/>
     </row>
@@ -3446,31 +3450,31 @@
     <row r="11" spans="1:3">
       <c r="A11" s="4"/>
       <c r="B11" s="95" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="97" t="s">
         <v>72</v>
-      </c>
-      <c r="C11" s="97" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" thickBot="1">
       <c r="A12" s="4"/>
       <c r="B12" s="95"/>
       <c r="C12" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" thickBot="1">
       <c r="A13" s="4"/>
       <c r="B13" s="95"/>
       <c r="C13" s="98" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="4"/>
       <c r="B14" s="95"/>
       <c r="C14" s="96" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -3481,59 +3485,59 @@
     <row r="16" spans="1:3">
       <c r="A16" s="4"/>
       <c r="B16" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="99" t="s">
         <v>77</v>
-      </c>
-      <c r="C16" s="99" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="4"/>
       <c r="B17" s="95"/>
       <c r="C17" s="100" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="4"/>
       <c r="B18" s="95"/>
       <c r="C18" s="101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="4"/>
       <c r="B19" s="95"/>
       <c r="C19" s="102" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="4"/>
       <c r="B20" s="103"/>
       <c r="C20" s="104" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="4"/>
       <c r="B21" s="103"/>
       <c r="C21" s="105" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="4"/>
       <c r="B22" s="103"/>
       <c r="C22" s="106" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="4"/>
       <c r="B23" s="103"/>
       <c r="C23" s="107" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3549,23 +3553,23 @@
   </sheetPr>
   <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="3.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
@@ -3580,7 +3584,7 @@
     </row>
     <row r="2" spans="2:10">
       <c r="B2" s="200" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="201"/>
       <c r="D2" s="201"/>
@@ -3676,7 +3680,7 @@
     <row r="10" spans="2:10" s="2" customFormat="1" ht="19" thickBot="1">
       <c r="B10" s="35"/>
       <c r="C10" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="64"/>
       <c r="E10" s="19"/>
@@ -3702,7 +3706,7 @@
       <c r="G11" s="75"/>
       <c r="H11" s="63"/>
       <c r="I11" s="146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J11" s="18"/>
     </row>
@@ -3714,14 +3718,14 @@
       <c r="D12" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="29">
-        <v>0.98</v>
+      <c r="E12" s="72">
+        <v>1</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
-      <c r="I12" s="29" t="s">
-        <v>63</v>
+      <c r="I12" s="209" t="s">
+        <v>185</v>
       </c>
       <c r="J12" s="120"/>
     </row>
@@ -3788,7 +3792,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="72">
         <f>'Research data'!H7</f>
@@ -3800,7 +3804,7 @@
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J16" s="120"/>
     </row>
@@ -3810,7 +3814,7 @@
         <v>45</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="72">
         <v>0</v>
@@ -3821,7 +3825,7 @@
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="146" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J17" s="120"/>
     </row>
@@ -3839,7 +3843,7 @@
     <row r="19" spans="2:10" ht="17" thickBot="1">
       <c r="B19" s="30"/>
       <c r="C19" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="125"/>
       <c r="E19" s="55"/>
@@ -3867,7 +3871,7 @@
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J20" s="121"/>
     </row>
@@ -3888,7 +3892,7 @@
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="146" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J21" s="121"/>
     </row>
@@ -3910,7 +3914,7 @@
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="195" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J22" s="120"/>
     </row>
@@ -3927,7 +3931,7 @@
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="151" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="29" t="s">
@@ -3953,7 +3957,7 @@
       </c>
       <c r="H24" s="26"/>
       <c r="I24" s="146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J24" s="120"/>
     </row>
@@ -3975,7 +3979,7 @@
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J25" s="120"/>
     </row>
@@ -3996,7 +4000,7 @@
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="147" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J26" s="120"/>
     </row>
@@ -4017,7 +4021,7 @@
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="148" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J27" s="120"/>
     </row>
@@ -4082,7 +4086,7 @@
       </c>
       <c r="H31" s="26"/>
       <c r="I31" s="146" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J31" s="120"/>
     </row>
@@ -4126,7 +4130,7 @@
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="148" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J33" s="120"/>
     </row>
@@ -4405,24 +4409,24 @@
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="28" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="28" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="28" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="28" customWidth="1"/>
-    <col min="9" max="9" width="2.42578125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="28" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="28" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="28" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="28" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="28" customWidth="1"/>
+    <col min="9" max="9" width="2.5" style="28" customWidth="1"/>
+    <col min="10" max="10" width="1.83203125" style="28" customWidth="1"/>
     <col min="11" max="11" width="13" style="28" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" style="28" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" style="28" customWidth="1"/>
     <col min="13" max="13" width="13" style="28" customWidth="1"/>
-    <col min="14" max="14" width="2.140625" style="28" customWidth="1"/>
+    <col min="14" max="14" width="2.1640625" style="28" customWidth="1"/>
     <col min="15" max="15" width="55" style="28" customWidth="1"/>
-    <col min="16" max="16384" width="10.7109375" style="28"/>
+    <col min="16" max="16384" width="10.6640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="17" thickBot="1"/>
@@ -4445,7 +4449,7 @@
     <row r="3" spans="2:15" s="19" customFormat="1">
       <c r="B3" s="35"/>
       <c r="C3" s="112" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -4454,20 +4458,20 @@
       </c>
       <c r="G3" s="112"/>
       <c r="H3" s="112" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" s="112"/>
       <c r="J3" s="112"/>
       <c r="K3" s="112" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L3" s="112"/>
       <c r="M3" s="112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N3" s="112"/>
       <c r="O3" s="112" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="2:15">
@@ -4489,7 +4493,7 @@
     <row r="5" spans="2:15" ht="17" thickBot="1">
       <c r="B5" s="30"/>
       <c r="C5" s="66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="66"/>
       <c r="E5" s="66"/>
@@ -4503,7 +4507,7 @@
     <row r="6" spans="2:15" ht="17" thickBot="1">
       <c r="B6" s="30"/>
       <c r="C6" s="142" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="66"/>
@@ -4531,7 +4535,7 @@
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
       <c r="F7" s="143" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="113"/>
       <c r="H7" s="182">
@@ -4545,7 +4549,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="151" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -4557,7 +4561,7 @@
       <c r="I8" s="44"/>
       <c r="J8" s="44"/>
       <c r="O8" s="151" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="17" thickBot="1">
@@ -4623,7 +4627,7 @@
     <row r="12" spans="2:15" ht="17" thickBot="1">
       <c r="B12" s="30"/>
       <c r="C12" s="117" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
@@ -4642,7 +4646,7 @@
         <v>0.2</v>
       </c>
       <c r="O12" s="165" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="2:15">
@@ -4660,7 +4664,7 @@
     <row r="14" spans="2:15" ht="17" thickBot="1">
       <c r="B14" s="30"/>
       <c r="C14" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -4674,7 +4678,7 @@
     <row r="15" spans="2:15" ht="17" thickBot="1">
       <c r="B15" s="30"/>
       <c r="C15" s="110" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -4704,7 +4708,7 @@
       <c r="D16" s="50"/>
       <c r="E16" s="50"/>
       <c r="F16" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G16" s="113"/>
       <c r="H16" s="49">
@@ -4724,12 +4728,12 @@
     <row r="17" spans="2:15" ht="17" thickBot="1">
       <c r="B17" s="30"/>
       <c r="C17" s="141" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="51"/>
       <c r="F17" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="113"/>
       <c r="H17" s="44"/>
@@ -4745,12 +4749,12 @@
     <row r="18" spans="2:15" ht="17" thickBot="1">
       <c r="B18" s="30"/>
       <c r="C18" s="141" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="51"/>
       <c r="F18" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G18" s="113"/>
       <c r="H18" s="44"/>
@@ -4766,12 +4770,12 @@
     <row r="19" spans="2:15" ht="17" thickBot="1">
       <c r="B19" s="30"/>
       <c r="C19" s="141" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="52"/>
       <c r="E19" s="52"/>
       <c r="F19" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="113"/>
       <c r="H19" s="44"/>
@@ -4787,7 +4791,7 @@
     <row r="20" spans="2:15" ht="17" thickBot="1">
       <c r="B20" s="30"/>
       <c r="C20" s="191" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D20" s="52"/>
       <c r="E20" s="52"/>
@@ -4806,18 +4810,18 @@
       </c>
       <c r="L20" s="44"/>
       <c r="O20" s="194" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="17" thickBot="1">
       <c r="B21" s="30"/>
       <c r="C21" s="191" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D21" s="52"/>
       <c r="E21" s="52"/>
       <c r="F21" s="193" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G21" s="113"/>
       <c r="H21" s="44"/>
@@ -4833,7 +4837,7 @@
     <row r="22" spans="2:15" ht="17" thickBot="1">
       <c r="B22" s="30"/>
       <c r="C22" s="116" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="53"/>
       <c r="E22" s="53"/>
@@ -4856,12 +4860,12 @@
     <row r="23" spans="2:15" ht="17" thickBot="1">
       <c r="B23" s="30"/>
       <c r="C23" s="116" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
       <c r="F23" s="109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G23" s="113"/>
       <c r="H23" s="46">
@@ -4954,18 +4958,18 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="81" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="81" customWidth="1"/>
     <col min="2" max="2" width="3" style="81" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="81" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="81" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="81" customWidth="1"/>
     <col min="5" max="5" width="14" style="81" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="81" customWidth="1"/>
-    <col min="7" max="8" width="12.7109375" style="82" customWidth="1"/>
-    <col min="9" max="9" width="32.42578125" style="82" customWidth="1"/>
-    <col min="10" max="10" width="76.42578125" style="81" customWidth="1"/>
-    <col min="11" max="16384" width="33.140625" style="81"/>
+    <col min="6" max="6" width="13.33203125" style="81" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="82" customWidth="1"/>
+    <col min="9" max="9" width="32.5" style="82" customWidth="1"/>
+    <col min="10" max="10" width="76.5" style="81" customWidth="1"/>
+    <col min="11" max="16384" width="33.1640625" style="81"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
@@ -5013,10 +5017,10 @@
         <v>33</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>18</v>
@@ -5039,25 +5043,25 @@
         <v>6</v>
       </c>
       <c r="D7" s="140" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="140" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="140" t="s">
+      <c r="F7" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="150" t="s">
+      <c r="G7" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="150" t="s">
+      <c r="H7" s="150" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="138" t="s">
         <v>111</v>
-      </c>
-      <c r="H7" s="150" t="s">
-        <v>110</v>
-      </c>
-      <c r="I7" s="139" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" s="138" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="8" spans="2:11">
@@ -5084,7 +5088,7 @@
     <row r="11" spans="2:11">
       <c r="B11" s="86"/>
       <c r="C11" s="149" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" s="82"/>
     </row>
@@ -5117,10 +5121,10 @@
     <row r="16" spans="2:11">
       <c r="B16" s="86"/>
       <c r="C16" s="167" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="167" t="s">
         <v>108</v>
-      </c>
-      <c r="D16" s="167" t="s">
-        <v>109</v>
       </c>
       <c r="E16" s="183">
         <v>43076</v>
@@ -5130,32 +5134,32 @@
       </c>
       <c r="G16" s="167"/>
       <c r="H16" s="167" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" s="167" t="s">
         <v>139</v>
-      </c>
-      <c r="I16" s="167" t="s">
-        <v>140</v>
       </c>
       <c r="J16" s="88"/>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="86"/>
       <c r="C17" s="166" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" s="167" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" s="167">
         <v>2018</v>
       </c>
       <c r="F17" s="168" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="168" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="168" t="s">
+      <c r="H17" s="169" t="s">
         <v>127</v>
-      </c>
-      <c r="H17" s="169" t="s">
-        <v>128</v>
       </c>
       <c r="J17" s="90"/>
     </row>
@@ -5171,11 +5175,11 @@
     <row r="20" spans="2:10">
       <c r="B20" s="86"/>
       <c r="C20" s="167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D20" s="167"/>
       <c r="E20" s="167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F20" s="189">
         <v>2017</v>
@@ -5185,7 +5189,7 @@
         <v>2019</v>
       </c>
       <c r="I20" s="167" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J20" s="167"/>
     </row>
@@ -5198,20 +5202,20 @@
       <c r="G21" s="190"/>
       <c r="H21" s="167"/>
       <c r="I21" s="167" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J21" s="167"/>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="86"/>
       <c r="C22" s="196" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="196" t="s">
         <v>180</v>
       </c>
-      <c r="D22" s="196" t="s">
-        <v>181</v>
-      </c>
       <c r="E22" s="196" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F22" s="197">
         <v>2019</v>
@@ -5223,10 +5227,10 @@
         <v>2019</v>
       </c>
       <c r="I22" s="199" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" s="196" t="s">
         <v>182</v>
-      </c>
-      <c r="J22" s="196" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -5317,14 +5321,14 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="127" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="127" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="127" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="127" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="127" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="127" customWidth="1"/>
     <col min="4" max="4" width="34" style="127" customWidth="1"/>
     <col min="5" max="5" width="23" style="127" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="127"/>
+    <col min="6" max="16384" width="10.6640625" style="127"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="17" thickBot="1"/>
@@ -5349,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -5369,7 +5373,7 @@
     <row r="5" spans="2:14">
       <c r="B5" s="134"/>
       <c r="C5" s="167" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N5" s="135"/>
     </row>
@@ -5431,7 +5435,7 @@
     <row r="18" spans="2:14">
       <c r="B18" s="134"/>
       <c r="C18" s="167" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N18" s="135"/>
     </row>
@@ -5450,7 +5454,7 @@
     <row r="21" spans="2:14" s="167" customFormat="1">
       <c r="B21" s="171"/>
       <c r="C21" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="172"/>
       <c r="E21" s="172"/>
@@ -5469,13 +5473,13 @@
     <row r="23" spans="2:14" s="167" customFormat="1">
       <c r="B23" s="171"/>
       <c r="D23" s="172" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E23" s="172">
         <v>20</v>
       </c>
       <c r="F23" s="172" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G23" s="172"/>
       <c r="N23" s="173"/>
@@ -5488,7 +5492,7 @@
         <v>20000</v>
       </c>
       <c r="F24" s="172" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G24" s="172"/>
       <c r="N24" s="173"/>
@@ -5536,13 +5540,13 @@
     <row r="30" spans="2:14" s="167" customFormat="1">
       <c r="B30" s="171"/>
       <c r="C30" s="167" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D30" s="172"/>
       <c r="E30" s="172"/>
       <c r="F30" s="172"/>
       <c r="G30" s="172" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N30" s="173"/>
     </row>
@@ -5573,13 +5577,13 @@
     <row r="34" spans="2:22" s="167" customFormat="1">
       <c r="B34" s="171"/>
       <c r="D34" s="172" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E34" s="177">
         <v>40000</v>
       </c>
       <c r="F34" s="172" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G34" s="172"/>
       <c r="N34" s="173"/>
@@ -5587,13 +5591,13 @@
     <row r="35" spans="2:22" s="167" customFormat="1">
       <c r="B35" s="171"/>
       <c r="D35" s="172" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E35" s="177">
         <v>600000000</v>
       </c>
       <c r="F35" s="172" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G35" s="172"/>
       <c r="N35" s="173"/>
@@ -5617,13 +5621,13 @@
     <row r="38" spans="2:22" s="167" customFormat="1">
       <c r="B38" s="171"/>
       <c r="D38" s="172" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" s="178">
         <v>10</v>
       </c>
       <c r="F38" s="178" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G38" s="172"/>
       <c r="N38" s="173"/>
@@ -5631,14 +5635,14 @@
     <row r="39" spans="2:22" s="167" customFormat="1">
       <c r="B39" s="171"/>
       <c r="D39" s="172" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E39" s="179">
         <f>E38*E24</f>
         <v>200000</v>
       </c>
       <c r="F39" s="178" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G39" s="172"/>
       <c r="N39" s="173"/>
@@ -5646,7 +5650,7 @@
     <row r="40" spans="2:22" s="167" customFormat="1">
       <c r="B40" s="171"/>
       <c r="D40" s="172" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E40" s="180">
         <f>E39/1000000</f>
@@ -5785,14 +5789,14 @@
     <row r="56" spans="2:14">
       <c r="B56" s="134"/>
       <c r="C56" s="167" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N56" s="135"/>
     </row>
     <row r="57" spans="2:14">
       <c r="B57" s="134"/>
       <c r="D57" s="167" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N57" s="135"/>
     </row>
@@ -5822,7 +5826,7 @@
     <row r="60" spans="2:14">
       <c r="B60" s="134"/>
       <c r="D60" s="167" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E60" s="167">
         <f>AVERAGE(E58,E59)</f>
@@ -5869,17 +5873,17 @@
     <row r="70" spans="2:14">
       <c r="B70" s="134"/>
       <c r="C70" s="167" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N70" s="135"/>
     </row>
     <row r="71" spans="2:14">
       <c r="B71" s="134"/>
       <c r="D71" s="167" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" s="167" t="s">
         <v>144</v>
-      </c>
-      <c r="E71" s="167" t="s">
-        <v>145</v>
       </c>
       <c r="N71" s="135"/>
     </row>
@@ -6020,14 +6024,14 @@
       <c r="F103" s="172"/>
       <c r="G103" s="172"/>
       <c r="I103" s="172" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N103" s="173"/>
     </row>
     <row r="104" spans="2:14" s="167" customFormat="1">
       <c r="B104" s="171"/>
       <c r="C104" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D104" s="172"/>
       <c r="E104" s="172"/>
@@ -6042,21 +6046,21 @@
       <c r="F105" s="172"/>
       <c r="G105" s="172"/>
       <c r="K105" s="185" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L105" s="186">
         <f>0.83611</f>
         <v>0.83611000000000002</v>
       </c>
       <c r="M105" s="185" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N105" s="173"/>
     </row>
     <row r="106" spans="2:14" s="167" customFormat="1">
       <c r="B106" s="171"/>
       <c r="C106" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D106" s="172"/>
       <c r="E106" s="172"/>
@@ -6064,7 +6068,7 @@
       <c r="G106" s="172"/>
       <c r="K106" s="185"/>
       <c r="L106" s="187" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M106" s="185"/>
       <c r="N106" s="173"/>
@@ -6133,10 +6137,10 @@
     <row r="114" spans="2:14" s="167" customFormat="1">
       <c r="B114" s="171"/>
       <c r="C114" s="172" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D114" s="172" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E114" s="172"/>
       <c r="F114" s="172"/>
@@ -6147,20 +6151,20 @@
       <c r="B115" s="171"/>
       <c r="D115" s="172"/>
       <c r="E115" s="172" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F115" s="172">
         <v>871</v>
       </c>
       <c r="G115" s="172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N115" s="173"/>
     </row>
     <row r="116" spans="2:14" s="167" customFormat="1">
       <c r="B116" s="171"/>
       <c r="D116" s="172" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E116" s="172"/>
       <c r="F116" s="172"/>
@@ -6170,35 +6174,35 @@
     <row r="117" spans="2:14" s="167" customFormat="1">
       <c r="B117" s="171"/>
       <c r="D117" s="172" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E117" s="172"/>
       <c r="F117" s="172">
         <v>440</v>
       </c>
       <c r="G117" s="172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N117" s="173"/>
     </row>
     <row r="118" spans="2:14" s="167" customFormat="1">
       <c r="B118" s="171"/>
       <c r="D118" s="172" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E118" s="172"/>
       <c r="F118" s="172">
         <v>84</v>
       </c>
       <c r="G118" s="172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N118" s="173"/>
     </row>
     <row r="119" spans="2:14" s="167" customFormat="1">
       <c r="B119" s="171"/>
       <c r="D119" s="172" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E119" s="172"/>
       <c r="F119" s="172">
@@ -6206,28 +6210,28 @@
         <v>297</v>
       </c>
       <c r="G119" s="172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N119" s="173"/>
     </row>
     <row r="120" spans="2:14" s="167" customFormat="1">
       <c r="B120" s="171"/>
       <c r="D120" s="172" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E120" s="192"/>
       <c r="F120" s="167">
         <v>50</v>
       </c>
       <c r="G120" s="172" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N120" s="173"/>
     </row>
     <row r="121" spans="2:14" s="167" customFormat="1">
       <c r="B121" s="171"/>
       <c r="F121" s="167" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N121" s="173"/>
     </row>
@@ -6250,13 +6254,13 @@
     <row r="124" spans="2:14" s="167" customFormat="1">
       <c r="B124" s="171"/>
       <c r="D124" s="172" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E124" s="172">
         <v>14.7</v>
       </c>
       <c r="F124" s="172" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G124" s="172"/>
       <c r="N124" s="173"/>
@@ -6266,7 +6270,7 @@
       <c r="D125" s="172"/>
       <c r="E125" s="172"/>
       <c r="F125" s="172" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G125" s="172"/>
       <c r="N125" s="173"/>
@@ -6274,13 +6278,13 @@
     <row r="126" spans="2:14" s="167" customFormat="1">
       <c r="B126" s="171"/>
       <c r="D126" s="172" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E126" s="172">
         <v>30</v>
       </c>
       <c r="G126" s="172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N126" s="173"/>
     </row>
@@ -6295,14 +6299,14 @@
     <row r="128" spans="2:14" s="167" customFormat="1">
       <c r="B128" s="171"/>
       <c r="D128" s="172" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E128" s="172">
         <f>E124+(E126/E60)</f>
         <v>15.899999999999999</v>
       </c>
       <c r="F128" s="172" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G128" s="172"/>
       <c r="N128" s="173"/>
@@ -6386,7 +6390,7 @@
     <row r="141" spans="2:14">
       <c r="B141" s="134"/>
       <c r="D141" s="167" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N141" s="135"/>
     </row>

</xml_diff>